<commit_message>
Completion of Indicators chapter
- revision tbd
- no approval from supervisor
</commit_message>
<xml_diff>
--- a/BA_tex/tables/Indicators.xlsx
+++ b/BA_tex/tables/Indicators.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-3040" yWindow="-21360" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="-840" yWindow="-19240" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>INDICATORS</t>
   </si>
@@ -77,13 +77,6 @@
 events</t>
   </si>
   <si>
-    <t xml:space="preserve">no control flow but dependencies </t>
-  </si>
-  <si>
-    <t xml:space="preserve">decisions cannot be made without
-regarding interrelationships  </t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
@@ -92,15 +85,6 @@
   <si>
     <t xml:space="preserve">predefined, fully specified,
 repeatable, business process, control flow oriented </t>
-  </si>
-  <si>
-    <t xml:space="preserve">no control flow, knowledge driven,
-interdepended collaboration, 
-automation of data driven decisions </t>
-  </si>
-  <si>
-    <t>human decision-making, automated
-decision-making, dependency driven</t>
   </si>
   <si>
     <t>CMMN Spec
@@ -112,13 +96,6 @@
     <t xml:space="preserve">Does the work consist of routine elements which can be optimized or even automated? </t>
   </si>
   <si>
-    <t xml:space="preserve">Does the work consist of personnel making decisions across several departments or decisions that derive from spreadsheets? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">discounts which can be automated, complex decisions in oranizations
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">predefined sequences of
 activities with decisions (gateways), 
 to direct the sequence along the alternative 
@@ -155,8 +132,39 @@
   </si>
   <si>
     <t>Does the work comprise unstructured elements and 
-ad hoc worklfows requiring knowledge or 
+ad hoc workflows requiring knowledge or 
 experience instead of strict rules?</t>
+  </si>
+  <si>
+    <t>decisions only, but with all the requirements and input data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Detailed decision modeling and adjusting during run-time,
+Decision Requirements Graph and Decision Tables 
+realizing decision logic and involved authorities / dependencies </t>
+  </si>
+  <si>
+    <t>human decision-making, automated deicison making, 
+aggregation of knowledge, preparation of decisions</t>
+  </si>
+  <si>
+    <t>complex, data-centric, many requirements, engangement
+of human decision-makers</t>
+  </si>
+  <si>
+    <t>dependencies only</t>
+  </si>
+  <si>
+    <t>calculation of discount rates, salary, multi-instance decisions,
+cross divisional decisions involving several deciders, 
+aggregation of data to get a specific output for a specific case, 
+inter-divisional decision-making</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are there decisions that need to be adjusted during run-time, 
+are data-intensive or require the modeling of extra 
+information (policies, analytical models)
+or roles (responsible managers)? </t>
   </si>
 </sst>
 </file>
@@ -539,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -573,45 +581,47 @@
         <v>4</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="7" t="s">
+    </row>
+    <row r="6" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="80" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -619,10 +629,10 @@
         <v>14</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -633,10 +643,10 @@
         <v>10</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -644,13 +654,13 @@
         <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="112" x14ac:dyDescent="0.2">
@@ -661,24 +671,24 @@
         <v>13</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="80" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="112" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added process discovery and definition of terms
- Process discovery added
- definition of indicator terms
- refurbished indicators
- tables added and revised
</commit_message>
<xml_diff>
--- a/BA_tex/tables/Indicators.xlsx
+++ b/BA_tex/tables/Indicators.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27426"/>
-  <workbookPr/>
+  <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dominik/Google Drive/TUM/Semester 8 (drive)/Bachelorarbeit/bachelorthesis/BA_tex/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-840" yWindow="-19240" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -73,10 +73,6 @@
 workflows accross companies / departments etc.</t>
   </si>
   <si>
-    <t>simple driven by rules or 
-events</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
@@ -119,9 +115,6 @@
     <t>Ad hoc, not predefined, sparsely routine work</t>
   </si>
   <si>
-    <t>Stateful conditions, events, exit and entry criteria</t>
-  </si>
-  <si>
     <t>Not necessary but can be modeled</t>
   </si>
   <si>
@@ -165,13 +158,20 @@
 are data-intensive or require the modeling of extra 
 information (policies, analytical models)
 or roles (responsible managers)? </t>
+  </si>
+  <si>
+    <t>Stateful conditions, rules, exit and entry criteria</t>
+  </si>
+  <si>
+    <t>simple, driven by rules or 
+events</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -191,6 +191,12 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -547,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -581,44 +587,44 @@
         <v>4</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -626,13 +632,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -643,10 +649,10 @@
         <v>10</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -654,13 +660,13 @@
         <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="D9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="112" x14ac:dyDescent="0.2">
@@ -671,10 +677,10 @@
         <v>13</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="112" x14ac:dyDescent="0.2">
@@ -682,16 +688,18 @@
         <v>12</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>